<commit_message>
Arquivos rel analise web
</commit_message>
<xml_diff>
--- a/Teste_API/Casos de Teste API.xlsx
+++ b/Teste_API/Casos de Teste API.xlsx
@@ -5,13 +5,15 @@
   <sheets>
     <sheet state="visible" name="CT_API" sheetId="1" r:id="rId4"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">CT_API!$A$1:$I$175</definedName>
+  </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="246">
   <si>
     <t>X</t>
   </si>
@@ -711,7 +713,7 @@
   </si>
   <si>
     <t>Não exibe 202 nem 204, mas sim 201 que é associado a criação de registro.
-Exibiu 200 com texto de resposta "Created", essa combinaão acho indevida para esse caso de Delete.</t>
+Exibiu 201 com texto de resposta "Created", essa combinaão acho indevida para esse caso de Delete.</t>
   </si>
   <si>
     <t>Considerei um problema a descrição na espec. para esse item. 
@@ -971,6 +973,113 @@
 [] 
 ou exibir bookingid de outros registros que satisfaçam o critério.</t>
   </si>
+  <si>
+    <t>5. Relação dos testes que não passaram</t>
+  </si>
+  <si>
+    <t>Cenário</t>
+  </si>
+  <si>
+    <t>Nome da request</t>
+  </si>
+  <si>
+    <t>2.2.2.1 Criar uma nova reserva</t>
+  </si>
+  <si>
+    <t>2.2.2.1.b Criar uma Nova Reserva passando chekin maior checkout- CreateBooking - CNR-05_02_05</t>
+  </si>
+  <si>
+    <t>Verificar comportamento quando tenta criar uma Nova Reserva passando chekin maior checkout</t>
+  </si>
+  <si>
+    <t>Não deveria aceitar a criação do registro</t>
+  </si>
+  <si>
+    <t>Acatou e criou registro de reserva</t>
+  </si>
+  <si>
+    <t>Não deveria aceitar a criação do registro e com isso devolver Status Code diferente de 200 p.exe 500</t>
+  </si>
+  <si>
+    <t>Retonrou Status Code 200</t>
+  </si>
+  <si>
+    <t>2.2.2.1.c Criar uma Nova Reserva sem data chekin - CreateBooking - CNR-07_02_03_04</t>
+  </si>
+  <si>
+    <t>Verificar comportamento quando tenta criar nova reserva NÃO passando Data Checkin</t>
+  </si>
+  <si>
+    <t>Não deveria aceitar a criação do registro e com isso devolver não deveri retornar response com valores</t>
+  </si>
+  <si>
+    <t>Retornou response com valores semelhante a quando deveria criar o registro de reserva</t>
+  </si>
+  <si>
+    <t>2.2.2.4 Atualizar uma reserva existente</t>
+  </si>
+  <si>
+    <t>2.2.2.4.b Atualizar uma reserva existente - UpdateBooking - ARE-05-07-08</t>
+  </si>
+  <si>
+    <t>Atualizando uma reserva Deixando o nome em branco. Verificar se o campo "firstname" possui um valor diferente de vazio.</t>
+  </si>
+  <si>
+    <t>2.2.2.5 Deletar uma reserva</t>
+  </si>
+  <si>
+    <t>2.2.2.5 Deletar uma reserva - DeleteBooking - DR-03-04</t>
+  </si>
+  <si>
+    <t>Passar uma reserva existente para deletar.</t>
+  </si>
+  <si>
+    <t>Verificar o Schema da resposta. O schema dessa resposta deve ser (texto)</t>
+  </si>
+  <si>
+    <t>Verificar o Schema da resposta. O schema dessa resposta deve ser (texto): Created.
+Considero incorreto, no caso essa descrição, onde penso que deveria exibir algum texto fazendo menção a deltear o registro.
+*Teste de verificação dentro da requisição.</t>
+  </si>
+  <si>
+    <t>2.2.2.5.b Deletar uma Reserva - DeleteBooking - DR-07-08</t>
+  </si>
+  <si>
+    <t>Passar uma reserva INexistente para deletar.</t>
+  </si>
+  <si>
+    <t>idem anterior</t>
+  </si>
+  <si>
+    <t>2.2.3.2 Buscar reservas por data de check-in</t>
+  </si>
+  <si>
+    <t>2.2.3.2 Buscar reservas por data de check-in - GetBookingIds - BRCI-01</t>
+  </si>
+  <si>
+    <t>Passar data Checkin IGUAL Data cadastrada na criação da reserva.</t>
+  </si>
+  <si>
+    <t>2.2.3.2.d Buscar reservas por data do check-in INválidas- GetBookingIds - BRCI-07_02_04</t>
+  </si>
+  <si>
+    <t>Passar data Checkin inválida pex. 2023-02-31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.2.3.3 Buscar reservas por data de check-out </t>
+  </si>
+  <si>
+    <t>2.2.3.3.b Buscar reservas por data MENOS 1 DIA do check-out - GetBookingIds - BRCO-05</t>
+  </si>
+  <si>
+    <t>Passar data Checkout MENOR que a Data cadastrada/setada na criação da reserva.</t>
+  </si>
+  <si>
+    <t>2.2.3.3.c Buscar reservas por data MAIS 1 DIA do check-out - GetBookingIds - BRCO-06</t>
+  </si>
+  <si>
+    <t>Passar data Checkout MAIOR que a Data cadastrada/setada na criação da reserva.</t>
+  </si>
 </sst>
 </file>
 
@@ -993,7 +1102,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1016,6 +1125,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB7B7B7"/>
         <bgColor rgb="FFB7B7B7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9900"/>
+        <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
     <fill>
@@ -1045,7 +1160,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1079,13 +1194,16 @@
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
+    <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
     <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1308,8 +1426,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="2" width="3.88"/>
-    <col customWidth="1" min="3" max="3" width="14.0"/>
-    <col customWidth="1" min="4" max="4" width="34.75"/>
+    <col customWidth="1" min="3" max="3" width="14.88"/>
+    <col customWidth="1" min="4" max="4" width="88.25"/>
     <col customWidth="1" min="5" max="5" width="50.25"/>
     <col customWidth="1" min="6" max="6" width="38.88"/>
     <col customWidth="1" min="8" max="8" width="47.38"/>
@@ -3038,7 +3156,7 @@
         <v>0</v>
       </c>
       <c r="B45" s="1"/>
-      <c r="C45" s="8" t="s">
+      <c r="C45" s="11" t="s">
         <v>62</v>
       </c>
       <c r="D45" s="9" t="s">
@@ -3047,10 +3165,10 @@
       <c r="E45" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="F45" s="11" t="s">
+      <c r="F45" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="G45" s="12" t="s">
+      <c r="G45" s="13" t="s">
         <v>66</v>
       </c>
       <c r="H45" s="9" t="s">
@@ -3081,7 +3199,7 @@
         <v>0</v>
       </c>
       <c r="B46" s="1"/>
-      <c r="C46" s="8" t="s">
+      <c r="C46" s="11" t="s">
         <v>62</v>
       </c>
       <c r="D46" s="9" t="s">
@@ -3090,10 +3208,10 @@
       <c r="E46" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="F46" s="11" t="s">
+      <c r="F46" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="G46" s="12" t="s">
+      <c r="G46" s="13" t="s">
         <v>66</v>
       </c>
       <c r="H46" s="9" t="s">
@@ -3124,7 +3242,7 @@
         <v>0</v>
       </c>
       <c r="B47" s="1"/>
-      <c r="C47" s="8" t="s">
+      <c r="C47" s="11" t="s">
         <v>71</v>
       </c>
       <c r="D47" s="9" t="s">
@@ -3133,10 +3251,10 @@
       <c r="E47" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="F47" s="11" t="s">
+      <c r="F47" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="G47" s="12" t="s">
+      <c r="G47" s="13" t="s">
         <v>66</v>
       </c>
       <c r="H47" s="9" t="s">
@@ -3167,7 +3285,7 @@
         <v>0</v>
       </c>
       <c r="B48" s="1"/>
-      <c r="C48" s="8" t="s">
+      <c r="C48" s="11" t="s">
         <v>75</v>
       </c>
       <c r="D48" s="9" t="s">
@@ -3176,10 +3294,10 @@
       <c r="E48" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="F48" s="11" t="s">
+      <c r="F48" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="G48" s="12" t="s">
+      <c r="G48" s="13" t="s">
         <v>66</v>
       </c>
       <c r="H48" s="9" t="s">
@@ -3210,7 +3328,7 @@
         <v>0</v>
       </c>
       <c r="B49" s="1"/>
-      <c r="C49" s="8" t="s">
+      <c r="C49" s="11" t="s">
         <v>78</v>
       </c>
       <c r="D49" s="9" t="s">
@@ -3219,10 +3337,10 @@
       <c r="E49" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F49" s="11" t="s">
+      <c r="F49" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="G49" s="12" t="s">
+      <c r="G49" s="13" t="s">
         <v>66</v>
       </c>
       <c r="H49" s="9" t="s">
@@ -3989,22 +4107,22 @@
         <v>0</v>
       </c>
       <c r="B70" s="1"/>
-      <c r="C70" s="13" t="s">
+      <c r="C70" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D70" s="13" t="s">
+      <c r="D70" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E70" s="13" t="s">
+      <c r="E70" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="F70" s="13" t="s">
+      <c r="F70" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G70" s="13" t="s">
+      <c r="G70" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H70" s="13" t="s">
+      <c r="H70" s="14" t="s">
         <v>11</v>
       </c>
       <c r="I70" s="2"/>
@@ -4582,7 +4700,7 @@
       <c r="F85" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G85" s="12" t="s">
+      <c r="G85" s="13" t="s">
         <v>16</v>
       </c>
       <c r="H85" s="8" t="s">
@@ -4613,7 +4731,7 @@
         <v>0</v>
       </c>
       <c r="B86" s="1"/>
-      <c r="C86" s="8" t="s">
+      <c r="C86" s="11" t="s">
         <v>120</v>
       </c>
       <c r="D86" s="9" t="s">
@@ -4622,10 +4740,10 @@
       <c r="E86" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="F86" s="11" t="s">
+      <c r="F86" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G86" s="12" t="s">
+      <c r="G86" s="13" t="s">
         <v>66</v>
       </c>
       <c r="H86" s="9" t="s">
@@ -4668,7 +4786,7 @@
       <c r="F87" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G87" s="12" t="s">
+      <c r="G87" s="13" t="s">
         <v>16</v>
       </c>
       <c r="H87" s="8" t="s">
@@ -4699,7 +4817,7 @@
         <v>0</v>
       </c>
       <c r="B88" s="1"/>
-      <c r="C88" s="8" t="s">
+      <c r="C88" s="11" t="s">
         <v>126</v>
       </c>
       <c r="D88" s="9" t="s">
@@ -4708,10 +4826,10 @@
       <c r="E88" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="F88" s="12" t="s">
+      <c r="F88" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="G88" s="12" t="s">
+      <c r="G88" s="13" t="s">
         <v>66</v>
       </c>
       <c r="H88" s="9" t="s">
@@ -4742,7 +4860,7 @@
         <v>0</v>
       </c>
       <c r="B89" s="1"/>
-      <c r="C89" s="8" t="s">
+      <c r="C89" s="11" t="s">
         <v>130</v>
       </c>
       <c r="D89" s="9" t="s">
@@ -4751,10 +4869,10 @@
       <c r="E89" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="F89" s="11" t="s">
+      <c r="F89" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="G89" s="12" t="s">
+      <c r="G89" s="13" t="s">
         <v>66</v>
       </c>
       <c r="H89" s="9" t="s">
@@ -5077,7 +5195,7 @@
       <c r="F98" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G98" s="11" t="s">
+      <c r="G98" s="12" t="s">
         <v>16</v>
       </c>
       <c r="H98" s="8" t="s">
@@ -5108,7 +5226,7 @@
         <v>0</v>
       </c>
       <c r="B99" s="1"/>
-      <c r="C99" s="8" t="s">
+      <c r="C99" s="11" t="s">
         <v>139</v>
       </c>
       <c r="D99" s="8" t="s">
@@ -5117,10 +5235,10 @@
       <c r="E99" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="F99" s="11" t="s">
+      <c r="F99" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="G99" s="12" t="s">
+      <c r="G99" s="13" t="s">
         <v>66</v>
       </c>
       <c r="H99" s="9" t="s">
@@ -5151,7 +5269,7 @@
         <v>0</v>
       </c>
       <c r="B100" s="1"/>
-      <c r="C100" s="8" t="s">
+      <c r="C100" s="11" t="s">
         <v>143</v>
       </c>
       <c r="D100" s="8" t="s">
@@ -5160,10 +5278,10 @@
       <c r="E100" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="F100" s="11" t="s">
+      <c r="F100" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="G100" s="12" t="s">
+      <c r="G100" s="13" t="s">
         <v>66</v>
       </c>
       <c r="H100" s="9" t="s">
@@ -5206,7 +5324,7 @@
       <c r="F101" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="G101" s="12" t="s">
+      <c r="G101" s="13" t="s">
         <v>16</v>
       </c>
       <c r="H101" s="8" t="s">
@@ -5249,7 +5367,7 @@
       <c r="F102" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G102" s="12" t="s">
+      <c r="G102" s="13" t="s">
         <v>16</v>
       </c>
       <c r="H102" s="8" t="s">
@@ -5280,7 +5398,7 @@
         <v>0</v>
       </c>
       <c r="B103" s="1"/>
-      <c r="C103" s="8" t="s">
+      <c r="C103" s="11" t="s">
         <v>152</v>
       </c>
       <c r="D103" s="8" t="s">
@@ -5289,10 +5407,10 @@
       <c r="E103" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="F103" s="11" t="s">
+      <c r="F103" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="G103" s="12" t="s">
+      <c r="G103" s="13" t="s">
         <v>66</v>
       </c>
       <c r="H103" s="9" t="s">
@@ -5323,7 +5441,7 @@
         <v>0</v>
       </c>
       <c r="B104" s="1"/>
-      <c r="C104" s="8" t="s">
+      <c r="C104" s="11" t="s">
         <v>156</v>
       </c>
       <c r="D104" s="8" t="s">
@@ -5332,10 +5450,10 @@
       <c r="E104" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="F104" s="11" t="s">
+      <c r="F104" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="G104" s="12" t="s">
+      <c r="G104" s="13" t="s">
         <v>66</v>
       </c>
       <c r="H104" s="9" t="s">
@@ -5985,8 +6103,8 @@
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
-      <c r="E122" s="14"/>
-      <c r="F122" s="14"/>
+      <c r="E122" s="15"/>
+      <c r="F122" s="15"/>
       <c r="G122" s="2"/>
       <c r="H122" s="2"/>
       <c r="I122" s="2"/>
@@ -6057,7 +6175,7 @@
         <v>0</v>
       </c>
       <c r="B124" s="1"/>
-      <c r="C124" s="8" t="s">
+      <c r="C124" s="11" t="s">
         <v>176</v>
       </c>
       <c r="D124" s="9" t="s">
@@ -6066,10 +6184,10 @@
       <c r="E124" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="F124" s="11" t="s">
+      <c r="F124" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="G124" s="12" t="s">
+      <c r="G124" s="13" t="s">
         <v>66</v>
       </c>
       <c r="H124" s="8" t="s">
@@ -6315,7 +6433,7 @@
         <v>0</v>
       </c>
       <c r="B130" s="1"/>
-      <c r="C130" s="8" t="s">
+      <c r="C130" s="11" t="s">
         <v>188</v>
       </c>
       <c r="D130" s="9" t="s">
@@ -6324,10 +6442,10 @@
       <c r="E130" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="F130" s="11" t="s">
+      <c r="F130" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="G130" s="12" t="s">
+      <c r="G130" s="13" t="s">
         <v>66</v>
       </c>
       <c r="H130" s="9" t="s">
@@ -6358,7 +6476,7 @@
         <v>0</v>
       </c>
       <c r="B131" s="1"/>
-      <c r="C131" s="8" t="s">
+      <c r="C131" s="11" t="s">
         <v>188</v>
       </c>
       <c r="D131" s="8" t="s">
@@ -6367,10 +6485,10 @@
       <c r="E131" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="F131" s="11" t="s">
+      <c r="F131" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="G131" s="12" t="s">
+      <c r="G131" s="13" t="s">
         <v>66</v>
       </c>
       <c r="H131" s="9" t="s">
@@ -6402,9 +6520,9 @@
       </c>
       <c r="B132" s="1"/>
       <c r="C132" s="2"/>
-      <c r="D132" s="14"/>
-      <c r="E132" s="14"/>
-      <c r="F132" s="14"/>
+      <c r="D132" s="15"/>
+      <c r="E132" s="15"/>
+      <c r="F132" s="15"/>
       <c r="G132" s="2"/>
       <c r="H132" s="2"/>
       <c r="I132" s="2"/>
@@ -6433,9 +6551,9 @@
       </c>
       <c r="B133" s="1"/>
       <c r="C133" s="2"/>
-      <c r="D133" s="14"/>
-      <c r="E133" s="14"/>
-      <c r="F133" s="14"/>
+      <c r="D133" s="15"/>
+      <c r="E133" s="15"/>
+      <c r="F133" s="15"/>
       <c r="G133" s="2"/>
       <c r="H133" s="2"/>
       <c r="I133" s="2"/>
@@ -6566,8 +6684,8 @@
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
-      <c r="E137" s="14"/>
-      <c r="F137" s="14"/>
+      <c r="E137" s="15"/>
+      <c r="F137" s="15"/>
       <c r="G137" s="2"/>
       <c r="H137" s="2"/>
       <c r="I137" s="2"/>
@@ -6595,22 +6713,22 @@
         <v>0</v>
       </c>
       <c r="B138" s="1"/>
-      <c r="C138" s="13" t="s">
+      <c r="C138" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D138" s="13" t="s">
+      <c r="D138" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E138" s="13" t="s">
+      <c r="E138" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="F138" s="13" t="s">
+      <c r="F138" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G138" s="13" t="s">
+      <c r="G138" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H138" s="13" t="s">
+      <c r="H138" s="14" t="s">
         <v>11</v>
       </c>
       <c r="I138" s="2"/>
@@ -6810,7 +6928,7 @@
         <v>0</v>
       </c>
       <c r="B143" s="1"/>
-      <c r="C143" s="8" t="s">
+      <c r="C143" s="11" t="s">
         <v>204</v>
       </c>
       <c r="D143" s="9" t="s">
@@ -6819,10 +6937,10 @@
       <c r="E143" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="F143" s="11" t="s">
+      <c r="F143" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="G143" s="12" t="s">
+      <c r="G143" s="13" t="s">
         <v>66</v>
       </c>
       <c r="H143" s="9" t="s">
@@ -6853,7 +6971,7 @@
         <v>0</v>
       </c>
       <c r="B144" s="1"/>
-      <c r="C144" s="8" t="s">
+      <c r="C144" s="11" t="s">
         <v>208</v>
       </c>
       <c r="D144" s="9" t="s">
@@ -6862,10 +6980,10 @@
       <c r="E144" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="F144" s="11" t="s">
+      <c r="F144" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="G144" s="12" t="s">
+      <c r="G144" s="13" t="s">
         <v>66</v>
       </c>
       <c r="H144" s="9" t="s">
@@ -6892,14 +7010,16 @@
       <c r="AA144" s="2"/>
     </row>
     <row r="145">
-      <c r="A145" s="1"/>
+      <c r="A145" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B145" s="1"/>
       <c r="C145" s="2"/>
-      <c r="D145" s="14"/>
+      <c r="D145" s="15"/>
       <c r="E145" s="2"/>
-      <c r="F145" s="14"/>
+      <c r="F145" s="15"/>
       <c r="G145" s="6"/>
-      <c r="H145" s="14"/>
+      <c r="H145" s="15"/>
       <c r="I145" s="2"/>
       <c r="J145" s="2"/>
       <c r="K145" s="2"/>
@@ -6921,14 +7041,16 @@
       <c r="AA145" s="2"/>
     </row>
     <row r="146">
-      <c r="A146" s="2"/>
+      <c r="A146" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
       <c r="D146" s="2"/>
       <c r="E146" s="2"/>
       <c r="F146" s="2"/>
-      <c r="G146" s="2"/>
-      <c r="H146" s="2"/>
+      <c r="G146" s="1"/>
+      <c r="H146" s="1"/>
       <c r="I146" s="2"/>
       <c r="J146" s="2"/>
       <c r="K146" s="2"/>
@@ -6950,12 +7072,16 @@
       <c r="AA146" s="2"/>
     </row>
     <row r="147">
-      <c r="A147" s="2"/>
+      <c r="A147" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B147" s="2"/>
-      <c r="C147" s="2"/>
-      <c r="D147" s="2"/>
-      <c r="E147" s="2"/>
-      <c r="F147" s="2"/>
+      <c r="C147" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D147" s="4"/>
+      <c r="E147" s="4"/>
+      <c r="F147" s="4"/>
       <c r="G147" s="2"/>
       <c r="H147" s="2"/>
       <c r="I147" s="2"/>
@@ -6979,14 +7105,16 @@
       <c r="AA147" s="2"/>
     </row>
     <row r="148">
-      <c r="A148" s="2"/>
+      <c r="A148" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B148" s="2"/>
-      <c r="C148" s="2"/>
-      <c r="D148" s="2"/>
-      <c r="E148" s="2"/>
-      <c r="F148" s="14"/>
+      <c r="C148" s="5"/>
+      <c r="D148" s="6"/>
+      <c r="E148" s="6"/>
+      <c r="F148" s="6"/>
       <c r="G148" s="2"/>
-      <c r="H148" s="14"/>
+      <c r="H148" s="2"/>
       <c r="I148" s="2"/>
       <c r="J148" s="2"/>
       <c r="K148" s="2"/>
@@ -7008,15 +7136,29 @@
       <c r="AA148" s="2"/>
     </row>
     <row r="149">
-      <c r="A149" s="2"/>
+      <c r="A149" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B149" s="2"/>
-      <c r="C149" s="2"/>
-      <c r="D149" s="2"/>
-      <c r="E149" s="2"/>
-      <c r="F149" s="14"/>
-      <c r="G149" s="2"/>
-      <c r="H149" s="2"/>
-      <c r="I149" s="2"/>
+      <c r="C149" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="D149" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="E149" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F149" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G149" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H149" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I149" s="7"/>
       <c r="J149" s="2"/>
       <c r="K149" s="2"/>
       <c r="L149" s="2"/>
@@ -7037,15 +7179,29 @@
       <c r="AA149" s="2"/>
     </row>
     <row r="150">
-      <c r="A150" s="2"/>
+      <c r="A150" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B150" s="2"/>
-      <c r="C150" s="2"/>
-      <c r="D150" s="2"/>
-      <c r="E150" s="2"/>
-      <c r="F150" s="2"/>
-      <c r="G150" s="2"/>
-      <c r="H150" s="2"/>
-      <c r="I150" s="2"/>
+      <c r="C150" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D150" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="E150" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="F150" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="G150" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="H150" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I150" s="8"/>
       <c r="J150" s="2"/>
       <c r="K150" s="2"/>
       <c r="L150" s="2"/>
@@ -7066,15 +7222,29 @@
       <c r="AA150" s="2"/>
     </row>
     <row r="151">
-      <c r="A151" s="2"/>
+      <c r="A151" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B151" s="2"/>
-      <c r="C151" s="2"/>
-      <c r="D151" s="2"/>
-      <c r="E151" s="2"/>
-      <c r="F151" s="2"/>
-      <c r="G151" s="2"/>
-      <c r="H151" s="2"/>
-      <c r="I151" s="2"/>
+      <c r="C151" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D151" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E151" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F151" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="G151" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="H151" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I151" s="8"/>
       <c r="J151" s="2"/>
       <c r="K151" s="2"/>
       <c r="L151" s="2"/>
@@ -7095,15 +7265,29 @@
       <c r="AA151" s="2"/>
     </row>
     <row r="152">
-      <c r="A152" s="2"/>
+      <c r="A152" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B152" s="2"/>
-      <c r="C152" s="2"/>
-      <c r="D152" s="2"/>
-      <c r="E152" s="2"/>
-      <c r="F152" s="2"/>
-      <c r="G152" s="2"/>
-      <c r="H152" s="2"/>
-      <c r="I152" s="2"/>
+      <c r="C152" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D152" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="E152" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="F152" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="G152" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="H152" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I152" s="8"/>
       <c r="J152" s="2"/>
       <c r="K152" s="2"/>
       <c r="L152" s="2"/>
@@ -7124,15 +7308,29 @@
       <c r="AA152" s="2"/>
     </row>
     <row r="153">
-      <c r="A153" s="2"/>
+      <c r="A153" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B153" s="2"/>
-      <c r="C153" s="2"/>
-      <c r="D153" s="2"/>
-      <c r="E153" s="2"/>
-      <c r="F153" s="2"/>
-      <c r="G153" s="2"/>
-      <c r="H153" s="2"/>
-      <c r="I153" s="2"/>
+      <c r="C153" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D153" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E153" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F153" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="G153" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="H153" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I153" s="8"/>
       <c r="J153" s="2"/>
       <c r="K153" s="2"/>
       <c r="L153" s="2"/>
@@ -7153,15 +7351,29 @@
       <c r="AA153" s="2"/>
     </row>
     <row r="154">
-      <c r="A154" s="2"/>
+      <c r="A154" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B154" s="2"/>
-      <c r="C154" s="2"/>
-      <c r="D154" s="2"/>
-      <c r="E154" s="2"/>
-      <c r="F154" s="2"/>
-      <c r="G154" s="2"/>
-      <c r="H154" s="2"/>
-      <c r="I154" s="2"/>
+      <c r="C154" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D154" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E154" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F154" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="G154" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="H154" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I154" s="8"/>
       <c r="J154" s="2"/>
       <c r="K154" s="2"/>
       <c r="L154" s="2"/>
@@ -7182,15 +7394,27 @@
       <c r="AA154" s="2"/>
     </row>
     <row r="155">
-      <c r="A155" s="2"/>
+      <c r="A155" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B155" s="2"/>
-      <c r="C155" s="2"/>
-      <c r="D155" s="2"/>
-      <c r="E155" s="2"/>
-      <c r="F155" s="2"/>
-      <c r="G155" s="2"/>
-      <c r="H155" s="2"/>
-      <c r="I155" s="2"/>
+      <c r="C155" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="D155" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="E155" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="F155" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="G155" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="H155" s="8"/>
+      <c r="I155" s="8"/>
       <c r="J155" s="2"/>
       <c r="K155" s="2"/>
       <c r="L155" s="2"/>
@@ -7211,15 +7435,27 @@
       <c r="AA155" s="2"/>
     </row>
     <row r="156">
-      <c r="A156" s="2"/>
+      <c r="A156" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B156" s="2"/>
-      <c r="C156" s="2"/>
-      <c r="D156" s="2"/>
-      <c r="E156" s="2"/>
-      <c r="F156" s="2"/>
-      <c r="G156" s="2"/>
-      <c r="H156" s="2"/>
-      <c r="I156" s="2"/>
+      <c r="C156" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D156" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E156" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F156" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G156" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="H156" s="8"/>
+      <c r="I156" s="8"/>
       <c r="J156" s="2"/>
       <c r="K156" s="2"/>
       <c r="L156" s="2"/>
@@ -7240,15 +7476,27 @@
       <c r="AA156" s="2"/>
     </row>
     <row r="157">
-      <c r="A157" s="2"/>
+      <c r="A157" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B157" s="2"/>
-      <c r="C157" s="2"/>
-      <c r="D157" s="2"/>
-      <c r="E157" s="2"/>
-      <c r="F157" s="2"/>
-      <c r="G157" s="2"/>
-      <c r="H157" s="2"/>
-      <c r="I157" s="2"/>
+      <c r="C157" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D157" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E157" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F157" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G157" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="H157" s="8"/>
+      <c r="I157" s="8"/>
       <c r="J157" s="2"/>
       <c r="K157" s="2"/>
       <c r="L157" s="2"/>
@@ -7269,15 +7517,29 @@
       <c r="AA157" s="2"/>
     </row>
     <row r="158">
-      <c r="A158" s="2"/>
+      <c r="A158" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B158" s="2"/>
-      <c r="C158" s="2"/>
-      <c r="D158" s="2"/>
-      <c r="E158" s="2"/>
-      <c r="F158" s="2"/>
-      <c r="G158" s="2"/>
-      <c r="H158" s="2"/>
-      <c r="I158" s="2"/>
+      <c r="C158" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="D158" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="E158" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F158" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="G158" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="H158" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="I158" s="8"/>
       <c r="J158" s="2"/>
       <c r="K158" s="2"/>
       <c r="L158" s="2"/>
@@ -7298,15 +7560,29 @@
       <c r="AA158" s="2"/>
     </row>
     <row r="159">
-      <c r="A159" s="2"/>
+      <c r="A159" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B159" s="2"/>
-      <c r="C159" s="2"/>
-      <c r="D159" s="2"/>
-      <c r="E159" s="2"/>
-      <c r="F159" s="2"/>
-      <c r="G159" s="2"/>
-      <c r="H159" s="2"/>
-      <c r="I159" s="2"/>
+      <c r="C159" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D159" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E159" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="F159" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="G159" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="H159" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="I159" s="8"/>
       <c r="J159" s="2"/>
       <c r="K159" s="2"/>
       <c r="L159" s="2"/>
@@ -7327,15 +7603,29 @@
       <c r="AA159" s="2"/>
     </row>
     <row r="160">
-      <c r="A160" s="2"/>
+      <c r="A160" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B160" s="2"/>
-      <c r="C160" s="2"/>
-      <c r="D160" s="2"/>
-      <c r="E160" s="2"/>
-      <c r="F160" s="2"/>
-      <c r="G160" s="2"/>
-      <c r="H160" s="2"/>
-      <c r="I160" s="2"/>
+      <c r="C160" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D160" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="E160" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="F160" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="G160" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="H160" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="I160" s="8"/>
       <c r="J160" s="2"/>
       <c r="K160" s="2"/>
       <c r="L160" s="2"/>
@@ -7356,15 +7646,29 @@
       <c r="AA160" s="2"/>
     </row>
     <row r="161">
-      <c r="A161" s="2"/>
+      <c r="A161" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B161" s="2"/>
-      <c r="C161" s="2"/>
-      <c r="D161" s="2"/>
-      <c r="E161" s="2"/>
-      <c r="F161" s="2"/>
-      <c r="G161" s="2"/>
-      <c r="H161" s="2"/>
-      <c r="I161" s="2"/>
+      <c r="C161" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D161" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E161" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="F161" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="G161" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="H161" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="I161" s="8"/>
       <c r="J161" s="2"/>
       <c r="K161" s="2"/>
       <c r="L161" s="2"/>
@@ -7385,15 +7689,27 @@
       <c r="AA161" s="2"/>
     </row>
     <row r="162">
-      <c r="A162" s="2"/>
+      <c r="A162" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B162" s="2"/>
-      <c r="C162" s="2"/>
-      <c r="D162" s="2"/>
-      <c r="E162" s="2"/>
-      <c r="F162" s="2"/>
-      <c r="G162" s="2"/>
-      <c r="H162" s="2"/>
-      <c r="I162" s="2"/>
+      <c r="C162" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="D162" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="E162" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="F162" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="G162" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="H162" s="8"/>
+      <c r="I162" s="8"/>
       <c r="J162" s="2"/>
       <c r="K162" s="2"/>
       <c r="L162" s="2"/>
@@ -7414,15 +7730,29 @@
       <c r="AA162" s="2"/>
     </row>
     <row r="163">
-      <c r="A163" s="2"/>
+      <c r="A163" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B163" s="2"/>
-      <c r="C163" s="2"/>
-      <c r="D163" s="2"/>
-      <c r="E163" s="2"/>
-      <c r="F163" s="2"/>
-      <c r="G163" s="2"/>
-      <c r="H163" s="2"/>
-      <c r="I163" s="2"/>
+      <c r="C163" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D163" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="E163" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="F163" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="G163" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="H163" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="I163" s="8"/>
       <c r="J163" s="2"/>
       <c r="K163" s="2"/>
       <c r="L163" s="2"/>
@@ -7443,15 +7773,27 @@
       <c r="AA163" s="2"/>
     </row>
     <row r="164">
-      <c r="A164" s="2"/>
+      <c r="A164" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B164" s="2"/>
-      <c r="C164" s="2"/>
-      <c r="D164" s="2"/>
-      <c r="E164" s="2"/>
-      <c r="F164" s="2"/>
-      <c r="G164" s="2"/>
-      <c r="H164" s="2"/>
-      <c r="I164" s="2"/>
+      <c r="C164" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D164" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E164" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="F164" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="G164" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="H164" s="8"/>
+      <c r="I164" s="8"/>
       <c r="J164" s="2"/>
       <c r="K164" s="2"/>
       <c r="L164" s="2"/>
@@ -7472,15 +7814,29 @@
       <c r="AA164" s="2"/>
     </row>
     <row r="165">
-      <c r="A165" s="2"/>
+      <c r="A165" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B165" s="2"/>
-      <c r="C165" s="2"/>
-      <c r="D165" s="2"/>
-      <c r="E165" s="2"/>
-      <c r="F165" s="2"/>
-      <c r="G165" s="2"/>
-      <c r="H165" s="2"/>
-      <c r="I165" s="2"/>
+      <c r="C165" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="D165" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="E165" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="F165" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="G165" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="H165" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="I165" s="8"/>
       <c r="J165" s="2"/>
       <c r="K165" s="2"/>
       <c r="L165" s="2"/>
@@ -7501,15 +7857,29 @@
       <c r="AA165" s="2"/>
     </row>
     <row r="166">
-      <c r="A166" s="2"/>
+      <c r="A166" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B166" s="2"/>
-      <c r="C166" s="2"/>
-      <c r="D166" s="2"/>
-      <c r="E166" s="2"/>
-      <c r="F166" s="2"/>
-      <c r="G166" s="2"/>
-      <c r="H166" s="2"/>
-      <c r="I166" s="2"/>
+      <c r="C166" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D166" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="E166" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="F166" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="G166" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="H166" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="I166" s="8"/>
       <c r="J166" s="2"/>
       <c r="K166" s="2"/>
       <c r="L166" s="2"/>
@@ -7530,15 +7900,17 @@
       <c r="AA166" s="2"/>
     </row>
     <row r="167">
-      <c r="A167" s="2"/>
+      <c r="A167" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B167" s="2"/>
-      <c r="C167" s="2"/>
-      <c r="D167" s="2"/>
-      <c r="E167" s="2"/>
-      <c r="F167" s="2"/>
-      <c r="G167" s="2"/>
-      <c r="H167" s="2"/>
-      <c r="I167" s="2"/>
+      <c r="C167" s="8"/>
+      <c r="D167" s="8"/>
+      <c r="E167" s="9"/>
+      <c r="F167" s="9"/>
+      <c r="G167" s="9"/>
+      <c r="H167" s="8"/>
+      <c r="I167" s="8"/>
       <c r="J167" s="2"/>
       <c r="K167" s="2"/>
       <c r="L167" s="2"/>
@@ -7559,14 +7931,16 @@
       <c r="AA167" s="2"/>
     </row>
     <row r="168">
-      <c r="A168" s="2"/>
+      <c r="A168" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B168" s="2"/>
-      <c r="C168" s="2"/>
-      <c r="D168" s="2"/>
-      <c r="E168" s="2"/>
-      <c r="F168" s="2"/>
-      <c r="G168" s="2"/>
-      <c r="H168" s="2"/>
+      <c r="C168" s="8"/>
+      <c r="D168" s="9"/>
+      <c r="E168" s="9"/>
+      <c r="F168" s="9"/>
+      <c r="G168" s="8"/>
+      <c r="H168" s="8"/>
       <c r="I168" s="2"/>
       <c r="J168" s="2"/>
       <c r="K168" s="2"/>
@@ -7588,7 +7962,9 @@
       <c r="AA168" s="2"/>
     </row>
     <row r="169">
-      <c r="A169" s="2"/>
+      <c r="A169" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B169" s="2"/>
       <c r="C169" s="2"/>
       <c r="D169" s="2"/>
@@ -7617,7 +7993,9 @@
       <c r="AA169" s="2"/>
     </row>
     <row r="170">
-      <c r="A170" s="2"/>
+      <c r="A170" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B170" s="2"/>
       <c r="C170" s="2"/>
       <c r="D170" s="2"/>
@@ -7646,7 +8024,9 @@
       <c r="AA170" s="2"/>
     </row>
     <row r="171">
-      <c r="A171" s="2"/>
+      <c r="A171" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B171" s="2"/>
       <c r="C171" s="2"/>
       <c r="D171" s="2"/>
@@ -7675,7 +8055,9 @@
       <c r="AA171" s="2"/>
     </row>
     <row r="172">
-      <c r="A172" s="2"/>
+      <c r="A172" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B172" s="2"/>
       <c r="C172" s="2"/>
       <c r="D172" s="2"/>
@@ -7704,7 +8086,9 @@
       <c r="AA172" s="2"/>
     </row>
     <row r="173">
-      <c r="A173" s="2"/>
+      <c r="A173" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B173" s="2"/>
       <c r="C173" s="2"/>
       <c r="D173" s="2"/>
@@ -7733,7 +8117,9 @@
       <c r="AA173" s="2"/>
     </row>
     <row r="174">
-      <c r="A174" s="2"/>
+      <c r="A174" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B174" s="2"/>
       <c r="C174" s="2"/>
       <c r="D174" s="2"/>
@@ -7762,7 +8148,9 @@
       <c r="AA174" s="2"/>
     </row>
     <row r="175">
-      <c r="A175" s="2"/>
+      <c r="A175" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B175" s="2"/>
       <c r="C175" s="2"/>
       <c r="D175" s="2"/>
@@ -7822,7 +8210,7 @@
     <row r="177">
       <c r="A177" s="2"/>
       <c r="B177" s="2"/>
-      <c r="C177" s="2"/>
+      <c r="C177" s="1"/>
       <c r="D177" s="2"/>
       <c r="E177" s="2"/>
       <c r="F177" s="2"/>
@@ -7851,7 +8239,7 @@
     <row r="178">
       <c r="A178" s="2"/>
       <c r="B178" s="2"/>
-      <c r="C178" s="2"/>
+      <c r="C178" s="1"/>
       <c r="D178" s="2"/>
       <c r="E178" s="2"/>
       <c r="F178" s="2"/>
@@ -7880,7 +8268,7 @@
     <row r="179">
       <c r="A179" s="2"/>
       <c r="B179" s="2"/>
-      <c r="C179" s="2"/>
+      <c r="C179" s="1"/>
       <c r="D179" s="2"/>
       <c r="E179" s="2"/>
       <c r="F179" s="2"/>
@@ -7909,7 +8297,7 @@
     <row r="180">
       <c r="A180" s="2"/>
       <c r="B180" s="2"/>
-      <c r="C180" s="2"/>
+      <c r="C180" s="1"/>
       <c r="D180" s="2"/>
       <c r="E180" s="2"/>
       <c r="F180" s="2"/>
@@ -7938,7 +8326,7 @@
     <row r="181">
       <c r="A181" s="2"/>
       <c r="B181" s="2"/>
-      <c r="C181" s="2"/>
+      <c r="C181" s="1"/>
       <c r="D181" s="2"/>
       <c r="E181" s="2"/>
       <c r="F181" s="2"/>
@@ -7967,7 +8355,7 @@
     <row r="182">
       <c r="A182" s="2"/>
       <c r="B182" s="2"/>
-      <c r="C182" s="2"/>
+      <c r="C182" s="1"/>
       <c r="D182" s="2"/>
       <c r="E182" s="2"/>
       <c r="F182" s="2"/>
@@ -7996,7 +8384,7 @@
     <row r="183">
       <c r="A183" s="2"/>
       <c r="B183" s="2"/>
-      <c r="C183" s="2"/>
+      <c r="C183" s="1"/>
       <c r="D183" s="2"/>
       <c r="E183" s="2"/>
       <c r="F183" s="2"/>
@@ -8025,7 +8413,7 @@
     <row r="184">
       <c r="A184" s="2"/>
       <c r="B184" s="2"/>
-      <c r="C184" s="2"/>
+      <c r="C184" s="1"/>
       <c r="D184" s="2"/>
       <c r="E184" s="2"/>
       <c r="F184" s="2"/>
@@ -8054,7 +8442,7 @@
     <row r="185">
       <c r="A185" s="2"/>
       <c r="B185" s="2"/>
-      <c r="C185" s="2"/>
+      <c r="C185" s="1"/>
       <c r="D185" s="2"/>
       <c r="E185" s="2"/>
       <c r="F185" s="2"/>
@@ -8083,7 +8471,7 @@
     <row r="186">
       <c r="A186" s="2"/>
       <c r="B186" s="2"/>
-      <c r="C186" s="2"/>
+      <c r="C186" s="1"/>
       <c r="D186" s="2"/>
       <c r="E186" s="2"/>
       <c r="F186" s="2"/>
@@ -8112,7 +8500,7 @@
     <row r="187">
       <c r="A187" s="2"/>
       <c r="B187" s="2"/>
-      <c r="C187" s="2"/>
+      <c r="C187" s="1"/>
       <c r="D187" s="2"/>
       <c r="E187" s="2"/>
       <c r="F187" s="2"/>
@@ -8141,7 +8529,7 @@
     <row r="188">
       <c r="A188" s="2"/>
       <c r="B188" s="2"/>
-      <c r="C188" s="2"/>
+      <c r="C188" s="1"/>
       <c r="D188" s="2"/>
       <c r="E188" s="2"/>
       <c r="F188" s="2"/>
@@ -8170,7 +8558,7 @@
     <row r="189">
       <c r="A189" s="2"/>
       <c r="B189" s="2"/>
-      <c r="C189" s="2"/>
+      <c r="C189" s="1"/>
       <c r="D189" s="2"/>
       <c r="E189" s="2"/>
       <c r="F189" s="2"/>
@@ -8199,7 +8587,7 @@
     <row r="190">
       <c r="A190" s="2"/>
       <c r="B190" s="2"/>
-      <c r="C190" s="2"/>
+      <c r="C190" s="1"/>
       <c r="D190" s="2"/>
       <c r="E190" s="2"/>
       <c r="F190" s="2"/>
@@ -8228,7 +8616,7 @@
     <row r="191">
       <c r="A191" s="2"/>
       <c r="B191" s="2"/>
-      <c r="C191" s="2"/>
+      <c r="C191" s="1"/>
       <c r="D191" s="2"/>
       <c r="E191" s="2"/>
       <c r="F191" s="2"/>
@@ -8257,7 +8645,7 @@
     <row r="192">
       <c r="A192" s="2"/>
       <c r="B192" s="2"/>
-      <c r="C192" s="2"/>
+      <c r="C192" s="1"/>
       <c r="D192" s="2"/>
       <c r="E192" s="2"/>
       <c r="F192" s="2"/>
@@ -8286,7 +8674,7 @@
     <row r="193">
       <c r="A193" s="2"/>
       <c r="B193" s="2"/>
-      <c r="C193" s="2"/>
+      <c r="C193" s="1"/>
       <c r="D193" s="2"/>
       <c r="E193" s="2"/>
       <c r="F193" s="2"/>
@@ -35311,94 +35699,8 @@
       <c r="Z1124" s="2"/>
       <c r="AA1124" s="2"/>
     </row>
-    <row r="1125">
-      <c r="A1125" s="2"/>
-      <c r="B1125" s="2"/>
-      <c r="C1125" s="2"/>
-      <c r="D1125" s="2"/>
-      <c r="E1125" s="2"/>
-      <c r="F1125" s="2"/>
-      <c r="G1125" s="2"/>
-      <c r="H1125" s="2"/>
-      <c r="I1125" s="2"/>
-      <c r="J1125" s="2"/>
-      <c r="K1125" s="2"/>
-      <c r="L1125" s="2"/>
-      <c r="M1125" s="2"/>
-      <c r="N1125" s="2"/>
-      <c r="O1125" s="2"/>
-      <c r="P1125" s="2"/>
-      <c r="Q1125" s="2"/>
-      <c r="R1125" s="2"/>
-      <c r="S1125" s="2"/>
-      <c r="T1125" s="2"/>
-      <c r="U1125" s="2"/>
-      <c r="V1125" s="2"/>
-      <c r="W1125" s="2"/>
-      <c r="X1125" s="2"/>
-      <c r="Y1125" s="2"/>
-      <c r="Z1125" s="2"/>
-      <c r="AA1125" s="2"/>
-    </row>
-    <row r="1126">
-      <c r="A1126" s="2"/>
-      <c r="B1126" s="2"/>
-      <c r="C1126" s="2"/>
-      <c r="D1126" s="2"/>
-      <c r="E1126" s="2"/>
-      <c r="F1126" s="2"/>
-      <c r="G1126" s="2"/>
-      <c r="H1126" s="2"/>
-      <c r="I1126" s="2"/>
-      <c r="J1126" s="2"/>
-      <c r="K1126" s="2"/>
-      <c r="L1126" s="2"/>
-      <c r="M1126" s="2"/>
-      <c r="N1126" s="2"/>
-      <c r="O1126" s="2"/>
-      <c r="P1126" s="2"/>
-      <c r="Q1126" s="2"/>
-      <c r="R1126" s="2"/>
-      <c r="S1126" s="2"/>
-      <c r="T1126" s="2"/>
-      <c r="U1126" s="2"/>
-      <c r="V1126" s="2"/>
-      <c r="W1126" s="2"/>
-      <c r="X1126" s="2"/>
-      <c r="Y1126" s="2"/>
-      <c r="Z1126" s="2"/>
-      <c r="AA1126" s="2"/>
-    </row>
-    <row r="1127">
-      <c r="A1127" s="2"/>
-      <c r="B1127" s="2"/>
-      <c r="C1127" s="2"/>
-      <c r="D1127" s="2"/>
-      <c r="E1127" s="2"/>
-      <c r="F1127" s="2"/>
-      <c r="G1127" s="2"/>
-      <c r="H1127" s="2"/>
-      <c r="I1127" s="2"/>
-      <c r="J1127" s="2"/>
-      <c r="K1127" s="2"/>
-      <c r="L1127" s="2"/>
-      <c r="M1127" s="2"/>
-      <c r="N1127" s="2"/>
-      <c r="O1127" s="2"/>
-      <c r="P1127" s="2"/>
-      <c r="Q1127" s="2"/>
-      <c r="R1127" s="2"/>
-      <c r="S1127" s="2"/>
-      <c r="T1127" s="2"/>
-      <c r="U1127" s="2"/>
-      <c r="V1127" s="2"/>
-      <c r="W1127" s="2"/>
-      <c r="X1127" s="2"/>
-      <c r="Y1127" s="2"/>
-      <c r="Z1127" s="2"/>
-      <c r="AA1127" s="2"/>
-    </row>
   </sheetData>
+  <autoFilter ref="$A$1:$I$175"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>